<commit_message>
fixed bug in excel file
</commit_message>
<xml_diff>
--- a/TransConnector Data.xlsx
+++ b/TransConnector Data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
   <si>
     <t>Location name</t>
   </si>
@@ -177,7 +177,7 @@
     <t>David</t>
   </si>
   <si>
-    <t>Wilson</t>
+    <t>Lee</t>
   </si>
   <si>
     <t>Mary</t>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>Suzuki</t>
-  </si>
-  <si>
-    <t>Lee</t>
   </si>
 </sst>
 </file>
@@ -898,7 +895,7 @@
         <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>